<commit_message>
forced text format in excel template for channels
</commit_message>
<xml_diff>
--- a/src/ESM.xlsx
+++ b/src/ESM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qr24461/.julia/dev/esm/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA4B62D-70B7-2D45-9894-28F91CCDC528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58B0938-62BA-6941-B525-5FB3A33BADC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="13560" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="13560" activeTab="3" xr2:uid="{7C37CC98-1F4A-4A36-93A3-A48642CDB423}"/>
   </bookViews>
   <sheets>
     <sheet name="Samples" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -455,30 +454,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2569E313-B3CC-438F-A253-EA0F3E8D819B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
@@ -490,9 +490,6 @@
       <c r="G1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -502,30 +499,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA707B9-0BE9-45E5-A5EE-A3873F0594F1}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -563,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED90973F-A7AD-4C45-9BA8-61879BED2320}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>